<commit_message>
Modifeied code to fit new table structure
Modified SQL statements in the IngredientDAL class to join together information from the ingredient_info and ingredient tables in order to properly get all ingredients, add ingredients, remove ingredients, increment ingredients, and decrement ingredients.
</commit_message>
<xml_diff>
--- a/sprints/Product Backlog.xlsx
+++ b/sprints/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0194197c910975a1/Desktop/CapstoneRecipePlanner/sprints/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea003fa8715b128d/Desktop/CapstoneRecipePlanner/sprints/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{E37EBA73-AC70-4990-93AE-760CDB473ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C57C09D2-6F9B-4BBA-98BC-EC2E955F13BA}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{E37EBA73-AC70-4990-93AE-760CDB473ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFF4B69C-5F39-4C56-B96B-584CB99E0A11}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>As a…</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>I can see what's available to use</t>
+  </si>
+  <si>
+    <t>Add all shopping list to pantry</t>
+  </si>
+  <si>
+    <t>Remove all ingredients needed to cook recipe after making it</t>
   </si>
 </sst>
 </file>
@@ -432,22 +438,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="16.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="48.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="74.88671875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="16.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="74.85546875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -461,7 +467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -475,7 +481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -489,7 +495,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -503,79 +509,99 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D9">
-    <sortCondition ref="A2:A9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D11">
+    <sortCondition ref="A2:A11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added stretch tasks to Sprint 4 Backlog
Added "Add Recipe" and "Share Recipe" stretch tasks to the sprint backlog with assigned team members. These tasks will be completed if time allows.
</commit_message>
<xml_diff>
--- a/sprints/Product Backlog.xlsx
+++ b/sprints/Product Backlog.xlsx
@@ -5,20 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea003fa8715b128d/Desktop/CapstoneRecipePlanner/sprints/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea003fa8715b128d/Desktop/School Work/Capstone/CapstoneRecipePlanner/sprints/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{E37EBA73-AC70-4990-93AE-760CDB473ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFF4B69C-5F39-4C56-B96B-584CB99E0A11}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="30" windowWidth="13575" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -441,7 +452,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>